<commit_message>
adicionada coleccion para guardar todo lo de la prediccion
</commit_message>
<xml_diff>
--- a/Api Rest ML Prediccion Clima/configuraciones/datasets/daily_weather - copia.xlsx
+++ b/Api Rest ML Prediccion Clima/configuraciones/datasets/daily_weather - copia.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\QiDimMak\Downloads\Playvox Test - SE 2020) (1) (1) (1) (1)\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E9403EB-7FD4-4D19-B406-419D15AF46FA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86F78538-FB93-4498-9455-A5F36B914E41}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19335" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="18020" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="daily_weather" sheetId="1" r:id="rId1"/>
@@ -96,10 +96,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -419,13 +420,13 @@
   </sheetPr>
   <dimension ref="A1:K12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A400" sqref="A13:XFD400"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -460,7 +461,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>0</v>
       </c>
@@ -495,7 +496,7 @@
         <v>36.160000000000402</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>1</v>
       </c>
@@ -520,9 +521,7 @@
       <c r="H3" s="2">
         <v>0</v>
       </c>
-      <c r="I3" s="2">
-        <v>0</v>
-      </c>
+      <c r="I3" s="3"/>
       <c r="J3" s="2">
         <v>24.3286972918022</v>
       </c>
@@ -530,7 +529,7 @@
         <v>19.426596798562102</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>2</v>
       </c>
@@ -552,11 +551,9 @@
       <c r="G4" s="2">
         <v>22.100967199999999</v>
       </c>
-      <c r="H4" s="2">
-        <v>0</v>
-      </c>
+      <c r="H4" s="2"/>
       <c r="I4" s="2">
-        <v>20</v>
+        <v>70</v>
       </c>
       <c r="J4" s="2">
         <v>8.9000000000000394</v>
@@ -565,7 +562,7 @@
         <v>14.46</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>3</v>
       </c>
@@ -587,12 +584,8 @@
       <c r="G5" s="2">
         <v>5.1900453602193704</v>
       </c>
-      <c r="H5" s="2">
-        <v>0</v>
-      </c>
-      <c r="I5" s="2">
-        <v>0</v>
-      </c>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
       <c r="J5" s="2">
         <v>12.1891018687644</v>
       </c>
@@ -600,7 +593,7 @@
         <v>12.7425473537618</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>4</v>
       </c>
@@ -635,7 +628,7 @@
         <v>76.740000000000407</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>5</v>
       </c>
@@ -670,7 +663,7 @@
         <v>33.930000000000199</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>6</v>
       </c>
@@ -705,7 +698,7 @@
         <v>21.385656725200899</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>7</v>
       </c>
@@ -740,7 +733,7 @@
         <v>74.9200000000004</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>8</v>
       </c>
@@ -775,7 +768,7 @@
         <v>24.030000000000399</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>9</v>
       </c>
@@ -810,7 +803,7 @@
         <v>68.050000000001205</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>10</v>
       </c>

</xml_diff>